<commit_message>
Completed sign_up testscript without payment
</commit_message>
<xml_diff>
--- a/testDatas/register_generatedData.xlsx
+++ b/testDatas/register_generatedData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMARTZero\STARZero\testDatas\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>LastName</t>
   </si>
@@ -75,12 +75,31 @@
   </si>
   <si>
     <t>test1234</t>
+  </si>
+  <si>
+    <t>Pasquale</t>
+  </si>
+  <si>
+    <t>Johnston</t>
+  </si>
+  <si>
+    <t>Carola</t>
+  </si>
+  <si>
+    <t>Wyman</t>
+  </si>
+  <si>
+    <t>kareem.denesik@hotmail.com</t>
+  </si>
+  <si>
+    <t>7043203860</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,8 +428,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -419,7 +438,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB0C87C-4116-4B63-9EF0-934C6847F0DC}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -427,66 +446,92 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.7109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="26.140625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.42578125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -507,39 +552,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.7109375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.28515625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.140625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.42578125"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
     </row>

</xml_diff>